<commit_message>
New Java Sdk added
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/_ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/_ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
   <si>
     <t>Add - Edit and Delete Position Category From Excel</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>Fill in the required information completely</t>
   </si>
 </sst>
 </file>
@@ -68,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,6 +198,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>